<commit_message>
Second Release (Change at Config)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmet.altin\Documents\UiPath\Regex_CV\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOS\Renova\UiPath-Personal-Project\Regex_CV\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5AF31B-7950-49E5-94C6-8A4C207DE746}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D1ECEB-863B-40A3-930A-0ECBE34F4EC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,19 +114,19 @@
     <t>PATHS NEED TO BE CONFIGURE</t>
   </si>
   <si>
-    <t>C:\Users\ahmet.altin\Documents\UiPath\Regex_CV\Data\CV</t>
-  </si>
-  <si>
-    <t>C:\Users\ahmet.altin\Documents\UiPath\Regex_CV\Data\Input\Patterns.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\ahmet.altin\Documents\UiPath\Regex_CV\Data\Output</t>
-  </si>
-  <si>
     <t>ArananBasliklar</t>
   </si>
   <si>
     <t>Email,DogumTarihi,Egitim,SonIsTecrube,Sonpozisyon,YabanciDil,YabanciDilSeviye,Sehir,Telefon,TecrubeYil,Bolum</t>
+  </si>
+  <si>
+    <t>C:\REPOS\Renova\UiPath-Personal-Project\Regex_CV\Data\Input\Patterns.xlsx</t>
+  </si>
+  <si>
+    <t>C:\REPOS\Renova\UiPath-Personal-Project\Regex_CV\Data\CV</t>
+  </si>
+  <si>
+    <t>C:\REPOS\Renova\UiPath-Personal-Project\Regex_CV\Data\Output</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -579,7 +579,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -587,7 +587,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -595,16 +595,16 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>